<commit_message>
admin page - teacher page
</commit_message>
<xml_diff>
--- a/public/Student Excel Template.xlsx
+++ b/public/Student Excel Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hehe\WebstormProjects\dp_management\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34ACA84E-0DF9-4D63-9D23-42AF6E7B4437}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA0DCCFB-5A56-4FE8-8AEF-E9889F84B129}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="1080" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Student" sheetId="1" r:id="rId1"/>
@@ -455,7 +455,7 @@
   <dimension ref="A1:D1014"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>

</xml_diff>